<commit_message>
Updated test CSV files, added lookup table for emission energies
</commit_message>
<xml_diff>
--- a/finalCode/baseStationCode/xRay/xrf_analysis/EmissionsTable.xlsx
+++ b/finalCode/baseStationCode/xRay/xrf_analysis/EmissionsTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\Documents\Code\Dubotics\XRFEnergyCalibration\XRFSpectroscopy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\Documents\Code\GitHub\2015-16\finalCode\baseStationCode\xRay\xrf_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="429" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="429"/>
   </bookViews>
   <sheets>
     <sheet name="Emissions By Atomic Number" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="111">
   <si>
     <t>X-Ray Data Booklet Table 1-2. Photon energies, in electron volts, of principal K-, L-, and M-shell emission lines.</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>Element Name</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,28 +857,28 @@
         <v>54.3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -889,28 +892,28 @@
         <v>108.5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -924,28 +927,28 @@
         <v>183.3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -959,28 +962,28 @@
         <v>277</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -994,28 +997,28 @@
         <v>392.4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1029,28 +1032,28 @@
         <v>524.9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1064,28 +1067,28 @@
         <v>676.8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1102,25 +1105,25 @@
         <v>848.6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1140,22 +1143,22 @@
         <v>1071.0999999999999</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1175,22 +1178,22 @@
         <v>1302.2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1210,22 +1213,22 @@
         <v>1557.45</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1245,22 +1248,22 @@
         <v>1835.94</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1280,22 +1283,22 @@
         <v>2139.1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1315,22 +1318,22 @@
         <v>2464.04</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1350,22 +1353,22 @@
         <v>2815.6</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1385,22 +1388,22 @@
         <v>3190.5</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1420,22 +1423,22 @@
         <v>3589.6</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1464,13 +1467,13 @@
         <v>344.9</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1499,13 +1502,13 @@
         <v>399.6</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1534,13 +1537,13 @@
         <v>458.4</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1569,13 +1572,13 @@
         <v>519.20000000000005</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1604,13 +1607,13 @@
         <v>582.79999999999995</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1639,13 +1642,13 @@
         <v>648.79999999999995</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1674,13 +1677,13 @@
         <v>718.5</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1709,13 +1712,13 @@
         <v>791.4</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1744,13 +1747,13 @@
         <v>868.8</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1779,13 +1782,13 @@
         <v>949.8</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1814,13 +1817,13 @@
         <v>1034.7</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1849,13 +1852,13 @@
         <v>1124.8</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1884,13 +1887,13 @@
         <v>1218.5</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1919,13 +1922,13 @@
         <v>1317</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1954,13 +1957,13 @@
         <v>1419.23</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1989,13 +1992,13 @@
         <v>1525.9</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2024,13 +2027,13 @@
         <v>1636.6</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2059,13 +2062,13 @@
         <v>1752.17</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2094,13 +2097,13 @@
         <v>1871.72</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2129,13 +2132,13 @@
         <v>1995.84</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2170,7 +2173,7 @@
         <v>2302.6999999999998</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2205,7 +2208,7 @@
         <v>2461.8000000000002</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2240,7 +2243,7 @@
         <v>2623.5</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2275,7 +2278,7 @@
         <v>2792</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2310,7 +2313,7 @@
         <v>2964.5</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2345,7 +2348,7 @@
         <v>3143.8</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2380,7 +2383,7 @@
         <v>3328.7</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2415,7 +2418,7 @@
         <v>3519.59</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2450,7 +2453,7 @@
         <v>3716.86</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2485,7 +2488,7 @@
         <v>3920.81</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2520,7 +2523,7 @@
         <v>4131.12</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2555,7 +2558,7 @@
         <v>4347.79</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2590,7 +2593,7 @@
         <v>4570.8999999999996</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2625,7 +2628,7 @@
         <v>4800.8999999999996</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2648,19 +2651,19 @@
         <v>4109.8999999999996</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2695,7 +2698,7 @@
         <v>5280.4</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2730,7 +2733,7 @@
         <v>5531.1</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2905,7 +2908,7 @@
         <v>6892</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3710,7 +3713,7 @@
         <v>15744</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3739,13 +3742,13 @@
         <v>13876</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J85" s="9">
         <v>16251</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -3774,13 +3777,13 @@
         <v>14316</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J86" s="9">
         <v>16770</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3815,7 +3818,7 @@
         <v>17303</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -3850,7 +3853,7 @@
         <v>17849</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -3879,13 +3882,13 @@
         <v>15713</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="J89" s="9">
         <v>18408</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4001,13 +4004,13 @@
         <v>70</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F93" s="7">
         <v>13944.1</v>
@@ -4025,7 +4028,7 @@
         <v>20784.8</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4036,13 +4039,13 @@
         <v>71</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F94" s="7">
         <v>14278.6</v>
@@ -4060,7 +4063,7 @@
         <v>21417.3</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -4071,13 +4074,13 @@
         <v>72</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="F95" s="7">
         <v>14617.2</v>
@@ -4095,7 +4098,7 @@
         <v>22065.200000000001</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -4115,8 +4118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D838"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D299" sqref="D299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15865,8 +15868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E618"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>